<commit_message>
OIE replaced with WOAH all Excels
</commit_message>
<xml_diff>
--- a/agents/AHFV/AHFV-Data-Contents.xlsx
+++ b/agents/AHFV/AHFV-Data-Contents.xlsx
@@ -51,7 +51,7 @@
     <t xml:space="preserve">text</t>
   </si>
   <si>
-    <t xml:space="preserve">This is not an agent/disease listed by the World Organisation for Animal Health (OIE). Geographical distribution can therefore not be mapped directly from any available reports. </t>
+    <t xml:space="preserve">This is not an agent/disease listed by the World Organisation for Animal Health (WOAH). Geographical distribution can therefore not be mapped directly from any available reports. </t>
   </si>
   <si>
     <t xml:space="preserve">sub-title</t>
@@ -207,7 +207,7 @@
     <t xml:space="preserve">Diagnosis</t>
   </si>
   <si>
-    <t xml:space="preserve">There are no OIE- recommended standard tests for AHV.</t>
+    <t xml:space="preserve">There are no WOAH- recommended standard tests for AHV.</t>
   </si>
   <si>
     <t xml:space="preserve">EFSA conducts regular systematic literature reviews covering peer-reviewed literature in English since 1970, covering diagnostic tests approved for use in the European Union (EU). </t>
@@ -471,7 +471,7 @@
     <t xml:space="preserve">ref001</t>
   </si>
   <si>
-    <t xml:space="preserve">OIE-WAHIS (OIE World Animal Health Information System)</t>
+    <t xml:space="preserve">WOAH-WAHIS (WOAH World Animal Health Information System)</t>
   </si>
   <si>
     <t xml:space="preserve">https://wahis.oie.int/</t>
@@ -498,7 +498,7 @@
     <t xml:space="preserve">ref005</t>
   </si>
   <si>
-    <t xml:space="preserve">OIE (World Organisation for Animal Health). Terrestrial Animal Health Code 2021. OIE, Paris, France</t>
+    <t xml:space="preserve">WOAH (World Organisation for Animal Health). Terrestrial Animal Health Code 2021. WOAH, Paris, France</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.oie.int/en/what-we-do/standards/codes-and-manuals/terrestrial-code-online-access/?id=169&amp;L=0&amp;htmfile=chapitre_notification.htm</t>
@@ -525,7 +525,7 @@
     <t xml:space="preserve">ref008</t>
   </si>
   <si>
-    <t xml:space="preserve">OIE (World Organisation for Animal Health) Technical Disease Card: African swine fever. 2021.</t>
+    <t xml:space="preserve">WOAH (World Organisation for Animal Health) Technical Disease Card: African swine fever. 2021.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.oie.int/app/uploads/2021/03/oie-african-swine-fever-technical-disease-card.pdf</t>
@@ -534,7 +534,7 @@
     <t xml:space="preserve">ref009</t>
   </si>
   <si>
-    <t xml:space="preserve">OIE (World Organisation for Animal Health), 2021. African Swine fever. Chapter 15.1. OIE Terrestrial Animal Health Code, Paris, France</t>
+    <t xml:space="preserve">WOAH (World Organisation for Animal Health), 2021. African Swine fever. Chapter 15.1. WOAH Terrestrial Animal Health Code, Paris, France</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.oie.int/fileadmin/Home/eng/Health_standards/tahc/current/chapitre_asf.pdf</t>
@@ -543,7 +543,7 @@
     <t xml:space="preserve">ref010</t>
   </si>
   <si>
-    <t xml:space="preserve">OIE (World Organisation for Animal Health), 2019. African Swine fever. Chapter 3.08.01. OIE Terrestrial Manual, Paris, France</t>
+    <t xml:space="preserve">WOAH (World Organisation for Animal Health), 2019. African Swine fever. Chapter 3.08.01. WOAH Terrestrial Manual, Paris, France</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.oie.int/fileadmin/Home/eng/Health_standards/tahm/3.08.01_ASF.pdf</t>

</xml_diff>

<commit_message>
improve naming convention - ExpInfections
</commit_message>
<xml_diff>
--- a/agents/AHFV/AHFV-Data-Contents.xlsx
+++ b/agents/AHFV/AHFV-Data-Contents.xlsx
@@ -84,7 +84,7 @@
     <t xml:space="preserve">You can download all data collected through systematic literature review {ref011:here}. Data fields are explained in this {ref012:read-me file}.</t>
   </si>
   <si>
-    <t xml:space="preserve">The review was last updated in January 2021. The complete list of references is available for download {ref013:here}. If important references to primary studies are missing, contact {ref004:animal-diseases@efsa.europa.eu}. The full review protocol can be downloaded  {ref007:here}.</t>
+    <t xml:space="preserve">The review was last updated in January 2022. The complete list of references is available for download {ref013:here}. If important references to primary studies are missing, contact {ref004:animal-diseases@efsa.europa.eu}. The full review protocol can be downloaded  {ref007:here}.</t>
   </si>
   <si>
     <t xml:space="preserve">map</t>
@@ -126,7 +126,7 @@
     <t xml:space="preserve">You can download all data collected through systematic literature review {ref014:here}. Data fields are explained in this {ref015:read-me file}.</t>
   </si>
   <si>
-    <t xml:space="preserve">*The review was last updated in January 2021. The complete list of references is available for download {ref016:here}. If important references to primary studies are missing, contact {ref004:animal-diseases@efsa.europa.eu}. The full review protocol can be downloaded  {ref007:here}.</t>
+    <t xml:space="preserve">*The review was last updated in January 2022. The complete list of references is available for download {ref016:here}. If important references to primary studies are missing, contact {ref004:animal-diseases@efsa.europa.eu}. The full review protocol can be downloaded  {ref007:here}.</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health</t>
@@ -138,7 +138,7 @@
     <t xml:space="preserve">HTML file</t>
   </si>
   <si>
-    <t xml:space="preserve">Impact-AHV.html</t>
+    <t xml:space="preserve">ExperimentalInfections-AHV.html</t>
   </si>
   <si>
     <t xml:space="preserve">Agent</t>
@@ -177,7 +177,7 @@
     <t xml:space="preserve">You can download all data collected through systematic literature review {ref017:here}. Data fields are explained in this {ref018:read-me file}.</t>
   </si>
   <si>
-    <t xml:space="preserve">*The review was last updated in January 2021. The complete list of references is available for download {ref019:here}. If important references to primary studies are missing, contact {ref004:animal-diseases@efsa.europa.eu}. The full review protocol can be downloaded  {ref007:here}.</t>
+    <t xml:space="preserve">*The review was last updated in January 2022. The complete list of references is available for download {ref019:here}. If important references to primary studies are missing, contact {ref004:animal-diseases@efsa.europa.eu}. The full review protocol can be downloaded  {ref007:here}.</t>
   </si>
   <si>
     <t xml:space="preserve">Survival-AHV.html</t>
@@ -234,7 +234,7 @@
     <t xml:space="preserve">You can download all data collected through systematic literature review {ref020:here}. Data fields are explained in this {ref021:read-me file}.</t>
   </si>
   <si>
-    <t xml:space="preserve">The review was last updated in January 2021. The complete list of references is available for download {ref022:here}. If important references to primary studies are missing, contact {ref004:animal-diseases@efsa.europa.eu}. The full review protocol can be downloaded  {ref007:here}.</t>
+    <t xml:space="preserve">The review was last updated in January 2022. The complete list of references is available for download {ref022:here}. If important references to primary studies are missing, contact {ref004:animal-diseases@efsa.europa.eu}. The full review protocol can be downloaded  {ref007:here}.</t>
   </si>
   <si>
     <t xml:space="preserve">Diagnostic-AHV.html</t>

</xml_diff>